<commit_message>
Gradient study edited, fieldpic with new version
</commit_message>
<xml_diff>
--- a/gradient_study/091614_study.xlsx
+++ b/gradient_study/091614_study.xlsx
@@ -38,7 +38,7 @@
     <t>cap change</t>
   </si>
   <si>
-    <t>cap change / B0</t>
+    <t>(cap change)/B0</t>
   </si>
   <si>
     <t>dBx/dx [uG/cm]</t>
@@ -206,7 +206,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>